<commit_message>
Update for self define height
</commit_message>
<xml_diff>
--- a/Individual Tree/DataTemplate.xlsx
+++ b/Individual Tree/DataTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/35baf9bfce3de29c/Program/GitHub/Spherical2TreeAttributes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/35baf9bfce3de29c/Program/GitHub/Spherical2TreeAttributes/Individual Tree/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="292" documentId="13_ncr:1_{515E2205-0DA0-4A66-934C-FABF355D0C23}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{FF509662-3D0E-4F67-861E-CFC5070428AE}"/>
+  <xr:revisionPtr revIDLastSave="317" documentId="13_ncr:1_{515E2205-0DA0-4A66-934C-FABF355D0C23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{01744067-B029-42E6-9EA3-87730C793A25}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="15600" windowHeight="19440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tree" sheetId="1" r:id="rId1"/>
@@ -34,57 +34,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>Plot</t>
-  </si>
-  <si>
-    <t>16TopY</t>
-  </si>
-  <si>
-    <t>16TopX</t>
-  </si>
-  <si>
-    <t>16BaseY</t>
-  </si>
-  <si>
-    <t>16BaseX</t>
-  </si>
-  <si>
-    <t>26BaseX</t>
-  </si>
-  <si>
-    <t>26BaseY</t>
-  </si>
-  <si>
-    <t>26TopX</t>
-  </si>
-  <si>
-    <t>26TopY</t>
-  </si>
-  <si>
-    <t>16LeftX</t>
-  </si>
-  <si>
-    <t>16RightY</t>
-  </si>
-  <si>
-    <t>16LeftY</t>
-  </si>
-  <si>
-    <t>16RightX</t>
-  </si>
-  <si>
-    <t>26LeftX</t>
-  </si>
-  <si>
-    <t>26LeftY</t>
-  </si>
-  <si>
-    <t>26RightX</t>
-  </si>
-  <si>
-    <t>26RightY</t>
   </si>
   <si>
     <t>Distance</t>
@@ -175,6 +127,64 @@
   <si>
     <t>North26</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>North</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1BaseX</t>
+  </si>
+  <si>
+    <t>1BaseY</t>
+  </si>
+  <si>
+    <t>1TopX</t>
+  </si>
+  <si>
+    <t>1TopY</t>
+  </si>
+  <si>
+    <t>2BaseX</t>
+  </si>
+  <si>
+    <t>2BaseY</t>
+  </si>
+  <si>
+    <t>2TopX</t>
+  </si>
+  <si>
+    <t>2TopY</t>
+  </si>
+  <si>
+    <t>1LeftX</t>
+  </si>
+  <si>
+    <t>1LeftY</t>
+  </si>
+  <si>
+    <t>1RightX</t>
+  </si>
+  <si>
+    <t>1RightY</t>
+  </si>
+  <si>
+    <t>2LeftX</t>
+  </si>
+  <si>
+    <t>2LeftY</t>
+  </si>
+  <si>
+    <t>2RightX</t>
+  </si>
+  <si>
+    <t>2RightY</t>
+  </si>
+  <si>
+    <t>1CamHT</t>
+  </si>
+  <si>
+    <t>2CamHT</t>
   </si>
 </sst>
 </file>
@@ -579,207 +589,170 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W8"/>
+  <dimension ref="A1:Z8"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="I21" sqref="I21"/>
+      <selection pane="bottomLeft" activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" customWidth="1"/>
-    <col min="2" max="2" width="3.5546875" customWidth="1"/>
-    <col min="3" max="6" width="7.109375" style="3" customWidth="1"/>
-    <col min="7" max="10" width="7.109375" style="4" customWidth="1"/>
-    <col min="11" max="14" width="7.109375" style="5" customWidth="1"/>
-    <col min="15" max="18" width="7.109375" style="6" customWidth="1"/>
-    <col min="19" max="20" width="7.77734375" style="7" customWidth="1"/>
-    <col min="21" max="22" width="5.77734375" style="7" customWidth="1"/>
-    <col min="23" max="23" width="7.77734375" style="7" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="2" max="2" width="3.5703125" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" customWidth="1"/>
+    <col min="5" max="8" width="7.140625" style="3" customWidth="1"/>
+    <col min="9" max="12" width="7.140625" style="4" customWidth="1"/>
+    <col min="13" max="16" width="7.140625" style="5" customWidth="1"/>
+    <col min="17" max="20" width="7.140625" style="6" customWidth="1"/>
+    <col min="21" max="21" width="8.7109375" style="7" customWidth="1"/>
+    <col min="22" max="22" width="7.140625" style="7" customWidth="1"/>
+    <col min="23" max="23" width="6.140625" style="7" customWidth="1"/>
+    <col min="24" max="25" width="6.42578125" style="7" customWidth="1"/>
+    <col min="26" max="26" width="8.42578125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:26">
       <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="P1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="V1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="W1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="X1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="4" t="s">
+      <c r="Y1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:26">
+      <c r="A2" t="s">
         <v>6</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="U1" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="V1" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="W1" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23">
-      <c r="A2" t="s">
-        <v>22</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="3">
-        <v>402</v>
-      </c>
-      <c r="D2" s="3">
-        <v>2065</v>
-      </c>
-      <c r="E2" s="3">
-        <v>512</v>
-      </c>
-      <c r="F2" s="3">
-        <v>183</v>
-      </c>
-      <c r="G2" s="4">
-        <v>404</v>
-      </c>
-      <c r="H2" s="4">
-        <v>2266</v>
-      </c>
-      <c r="I2" s="4">
-        <v>513</v>
-      </c>
-      <c r="J2" s="4">
-        <v>229</v>
-      </c>
-      <c r="K2" s="5">
-        <v>450</v>
-      </c>
-      <c r="L2" s="5">
-        <v>1482</v>
-      </c>
-      <c r="M2" s="5">
-        <v>520</v>
-      </c>
-      <c r="N2" s="5">
-        <v>1482</v>
-      </c>
-      <c r="O2" s="6">
-        <v>447</v>
-      </c>
-      <c r="P2" s="6">
-        <v>1971</v>
-      </c>
-      <c r="Q2" s="6">
-        <v>521</v>
-      </c>
-      <c r="R2" s="6">
-        <v>1971</v>
-      </c>
-      <c r="S2" s="7">
-        <v>1.3583412081834345</v>
-      </c>
-      <c r="T2" s="7">
-        <v>8.001548648627721E-2</v>
-      </c>
-      <c r="U2" s="7">
-        <v>7.6527071384650487</v>
-      </c>
-      <c r="V2" s="7">
-        <v>11.929210092679632</v>
-      </c>
-      <c r="W2" s="7">
-        <v>127.67001548648628</v>
-      </c>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:26">
       <c r="B3" s="16"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
       <c r="M3" s="12"/>
       <c r="N3" s="12"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
       <c r="Q3" s="13"/>
       <c r="R3" s="13"/>
-      <c r="S3" s="14"/>
-      <c r="T3" s="14"/>
+      <c r="S3" s="13"/>
+      <c r="T3" s="13"/>
       <c r="U3" s="14"/>
       <c r="V3" s="14"/>
       <c r="W3" s="14"/>
+      <c r="X3" s="14"/>
+      <c r="Y3" s="14"/>
+      <c r="Z3" s="14"/>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:26">
       <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:26">
       <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
     </row>
-    <row r="6" spans="1:23">
+    <row r="6" spans="1:26">
       <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:26">
       <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:26">
       <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -790,22 +763,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65E163E6-8531-4066-AAF9-26BBCF296AA9}">
-  <dimension ref="A1:Z2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="2" customWidth="1"/>
-    <col min="3" max="9" width="8.88671875" customWidth="1"/>
-    <col min="10" max="10" width="13.109375" customWidth="1"/>
-    <col min="11" max="11" width="8.88671875" style="2" customWidth="1"/>
-    <col min="12" max="18" width="8.88671875" customWidth="1"/>
-    <col min="19" max="19" width="13.5546875" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="2" customWidth="1"/>
+    <col min="3" max="9" width="8.85546875" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" style="2" customWidth="1"/>
+    <col min="12" max="18" width="8.85546875" customWidth="1"/>
+    <col min="19" max="19" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
@@ -813,69 +786,69 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="M1" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="N1" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="R1" t="s">
-        <v>36</v>
-      </c>
-      <c r="S1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:21">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2">
         <v>226</v>

</xml_diff>